<commit_message>
Se refinó el backlog
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Entender ejemplo Ruby</t>
   </si>
@@ -24,9 +24,6 @@
     <t xml:space="preserve">Generar preguntas </t>
   </si>
   <si>
-    <t>lógica de siguiente pregunta, guardar en json</t>
-  </si>
-  <si>
     <t>Entender respuestas</t>
   </si>
   <si>
@@ -52,6 +49,27 @@
   </si>
   <si>
     <t>investigar sobre módulos en Node</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Crear modelo, crear tipos, crear main</t>
+  </si>
+  <si>
+    <t>Queremos poner cada cosa como un módulo</t>
+  </si>
+  <si>
+    <t>lógica de siguiente pregunta, guardar en json, que haya preguntar de distinta dificultad</t>
+  </si>
+  <si>
+    <t>Hace la página de registración, que genere la url de cada cliente, que se mantenga el estado</t>
+  </si>
+  <si>
+    <t>Hacer una url tipo hello world que tenga un help</t>
+  </si>
+  <si>
+    <t>Cliente de prueba</t>
   </si>
 </sst>
 </file>
@@ -390,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C10"/>
+  <dimension ref="B2:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,58 +420,78 @@
     <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>11</v>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Me faltó el backlog XD
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Entender ejemplo Ruby</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Cliente de prueba</t>
+  </si>
+  <si>
+    <t>Started</t>
   </si>
 </sst>
 </file>
@@ -122,7 +125,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -411,10 +414,10 @@
   <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
@@ -456,6 +459,9 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -472,6 +478,9 @@
       <c r="C8" t="s">
         <v>16</v>
       </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -492,6 +501,9 @@
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -505,7 +517,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -517,7 +529,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Agregamos un log con appenders. - Separamos en modulos el log y arrancamos un dispatcher.
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Entender ejemplo Ruby</t>
   </si>
@@ -72,7 +72,16 @@
     <t>Cliente de prueba</t>
   </si>
   <si>
-    <t>Started</t>
+    <t>Hacer un log</t>
+  </si>
+  <si>
+    <t>De lo que se le envía al servidor</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Despacahar las urls</t>
   </si>
 </sst>
 </file>
@@ -411,16 +420,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D11"/>
+  <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -459,9 +469,6 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -504,6 +511,25 @@
       </c>
       <c r="D11" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
primera implementación de playerManger
permite persistir los jugadores en memoria a través del
defaultPersistenceProvider
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="15825" windowHeight="9855"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="15825" windowHeight="9855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Agregar jugadores" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Entender ejemplo Ruby</t>
   </si>
@@ -82,16 +82,36 @@
   </si>
   <si>
     <t>Despacahar las urls</t>
+  </si>
+  <si>
+    <t>poner htmls en archivos separados</t>
+  </si>
+  <si>
+    <t>poder configurar por medio de un json</t>
+  </si>
+  <si>
+    <t>generar clase que permisista los jugadores</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,13 +134,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -134,7 +157,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -422,11 +445,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
@@ -463,7 +486,7 @@
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
@@ -533,18 +556,45 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" location="'Agregar jugadores'!A1" display="Poder agregar jugadores"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -555,7 +605,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Se agrego un objeto game que sirve como facede del juego.
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="15825" windowHeight="9855" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="15825" windowHeight="9855"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Entender ejemplo Ruby</t>
   </si>
@@ -78,9 +78,6 @@
     <t>De lo que se le envía al servidor</t>
   </si>
   <si>
-    <t>Start</t>
-  </si>
-  <si>
     <t>Despacahar las urls</t>
   </si>
   <si>
@@ -90,10 +87,16 @@
     <t>poder configurar por medio de un json</t>
   </si>
   <si>
-    <t>generar clase que permisista los jugadores</t>
-  </si>
-  <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>generar clase que persista los jugadores</t>
+  </si>
+  <si>
+    <t>Notificar a los jugadores</t>
+  </si>
+  <si>
+    <t>A partir del player manager notificar a cada jugador con lo que corresponda</t>
   </si>
 </sst>
 </file>
@@ -143,7 +146,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -157,7 +160,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -443,13 +446,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D13"/>
+  <dimension ref="B2:D14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
@@ -549,10 +552,18 @@
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -567,23 +578,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -591,7 +602,7 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -605,7 +616,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrego el header al backlog y se prueba el commit
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Entender ejemplo Ruby</t>
   </si>
@@ -97,13 +97,22 @@
   </si>
   <si>
     <t>A partir del player manager notificar a cada jugador con lo que corresponda</t>
+  </si>
+  <si>
+    <t>To do</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +124,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,9 +158,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -446,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +477,21 @@
     <col min="3" max="3" width="67.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -467,7 +499,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -475,12 +510,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -488,7 +529,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -496,7 +540,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -504,7 +551,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -515,7 +565,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -523,7 +576,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -531,7 +587,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -539,7 +598,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
@@ -550,7 +612,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
@@ -558,7 +623,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
       <c r="B14" t="s">
         <v>25</v>
       </c>
@@ -571,6 +639,7 @@
     <hyperlink ref="B6" location="'Agregar jugadores'!A1" display="Poder agregar jugadores"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Se modifico el backlog.
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Entender ejemplo Ruby</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Queremos poner cada cosa como un módulo</t>
   </si>
   <si>
-    <t>lógica de siguiente pregunta, guardar en json, que haya preguntar de distinta dificultad</t>
-  </si>
-  <si>
     <t>Hace la página de registración, que genere la url de cada cliente, que se mantenga el estado</t>
   </si>
   <si>
@@ -106,6 +103,30 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Leader board</t>
+  </si>
+  <si>
+    <t>Muestra los puntajes parciales de todos los jugadores</t>
+  </si>
+  <si>
+    <t>Agregar los puntajes a los jugadores</t>
+  </si>
+  <si>
+    <t>Cuando se agrega un jugador empieza con 0. Y se pueden sumar o restar</t>
+  </si>
+  <si>
+    <t>lógica de siguiente pregunta, guardar en json, que haya preguntas de distinta dificultad</t>
+  </si>
+  <si>
+    <t>Enviarle preguntas a los jugadores</t>
+  </si>
+  <si>
+    <t>Enviarles un request con la pregunta a los jugadores</t>
+  </si>
+  <si>
+    <t>A partir de los response de los jugadores asignar los puntajes correspondientes</t>
   </si>
 </sst>
 </file>
@@ -464,28 +485,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="67.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -507,7 +528,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -517,6 +538,9 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -537,7 +561,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -559,7 +583,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -592,7 +616,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -603,10 +627,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
         <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -617,7 +641,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -628,10 +652,43 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
-        <v>26</v>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -658,20 +715,20 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Se envian preguntas a los clientes y se manejan niveles.
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="90" windowWidth="15825" windowHeight="9855"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Agregar jugadores" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>Entender ejemplo Ruby</t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>A partir de los response de los jugadores asignar los puntajes correspondientes</t>
+  </si>
+  <si>
+    <t>¿Configurar qué?</t>
+  </si>
+  <si>
+    <t>Agregar más preguntas</t>
+  </si>
+  <si>
+    <t>Y sus respuestas. También determinar el orden de los niveles.</t>
+  </si>
+  <si>
+    <t>Que muestre lo que se le preguntó y conteste algún valor hardcodeado</t>
   </si>
 </sst>
 </file>
@@ -485,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,6 +542,9 @@
       <c r="C3" t="s">
         <v>33</v>
       </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -541,6 +556,9 @@
       <c r="C4" t="s">
         <v>36</v>
       </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -563,6 +581,9 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -599,6 +620,9 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -610,6 +634,9 @@
       <c r="C10" t="s">
         <v>13</v>
       </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -618,6 +645,9 @@
       <c r="B11" t="s">
         <v>16</v>
       </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
@@ -657,6 +687,9 @@
       <c r="C14" t="s">
         <v>25</v>
       </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -668,6 +701,9 @@
       <c r="C15" t="s">
         <v>30</v>
       </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -679,8 +715,11 @@
       <c r="C16" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -689,6 +728,20 @@
       </c>
       <c r="C17" t="s">
         <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -702,10 +755,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C5"/>
+  <dimension ref="B3:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,17 +766,23 @@
     <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
- Agregue una pregunta mas.
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="15825" windowHeight="9855"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="15825" windowHeight="9795"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>Entender ejemplo Ruby</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>Que muestre lo que se le preguntó y conteste algún valor hardcodeado</t>
+  </si>
+  <si>
+    <t>Escribir un cliente perfecto</t>
+  </si>
+  <si>
+    <t>Que conteste bien todas las preguntas y tenga puntaje perfecto.</t>
   </si>
 </sst>
 </file>
@@ -497,9 +503,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -742,6 +748,17 @@
       </c>
       <c r="C18" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -758,7 +775,7 @@
   <dimension ref="B3:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Agregamos varios items al backlog y un cliente perfecto
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
-    <sheet name="Agregar jugadores" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t>Entender ejemplo Ruby</t>
   </si>
@@ -36,12 +34,6 @@
     <t>Poder agregar jugadores</t>
   </si>
   <si>
-    <t>Lógica de niveles</t>
-  </si>
-  <si>
-    <t>se tiene que poder pasar de nivel con un get a una url</t>
-  </si>
-  <si>
     <t>Conexión de test para los clientes</t>
   </si>
   <si>
@@ -78,18 +70,6 @@
     <t>Despacahar las urls</t>
   </si>
   <si>
-    <t>poner htmls en archivos separados</t>
-  </si>
-  <si>
-    <t>poder configurar por medio de un json</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>generar clase que persista los jugadores</t>
-  </si>
-  <si>
     <t>Notificar a los jugadores</t>
   </si>
   <si>
@@ -129,9 +109,6 @@
     <t>A partir de los response de los jugadores asignar los puntajes correspondientes</t>
   </si>
   <si>
-    <t>¿Configurar qué?</t>
-  </si>
-  <si>
     <t>Agregar más preguntas</t>
   </si>
   <si>
@@ -145,6 +122,66 @@
   </si>
   <si>
     <t>Que conteste bien todas las preguntas y tenga puntaje perfecto.</t>
+  </si>
+  <si>
+    <t>Ordenar el leaderboard</t>
+  </si>
+  <si>
+    <t>Por puntaje</t>
+  </si>
+  <si>
+    <t>Poner estado al juego</t>
+  </si>
+  <si>
+    <t>No debe arrancar de una sino cuando se le da start</t>
+  </si>
+  <si>
+    <t>Poner pausa</t>
+  </si>
+  <si>
+    <t>Y resume</t>
+  </si>
+  <si>
+    <t>Preguntas por query string</t>
+  </si>
+  <si>
+    <t>Por post de forma "pregunta=¿Qué día es hoy?"</t>
+  </si>
+  <si>
+    <t>Agregar preguntas</t>
+  </si>
+  <si>
+    <t>Colores primarios</t>
+  </si>
+  <si>
+    <t>Hacer perfiles</t>
+  </si>
+  <si>
+    <t>Además tener un perfil de práctica (sin puntos)</t>
+  </si>
+  <si>
+    <t>Cambiar el perfil mientras está en pausa</t>
+  </si>
+  <si>
+    <t>Agregar botón para ir al leadearboard</t>
+  </si>
+  <si>
+    <t>Después de haber sido agregado</t>
+  </si>
+  <si>
+    <t>Poder decir "paso"</t>
+  </si>
+  <si>
+    <t>Y que reste puntos pero tira la siguiente pregunta</t>
+  </si>
+  <si>
+    <t>Lógica de perfiles</t>
+  </si>
+  <si>
+    <t>A Adrián no le gustó</t>
+  </si>
+  <si>
+    <t>Mejorar css</t>
   </si>
 </sst>
 </file>
@@ -503,28 +540,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="84.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -535,7 +572,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -546,10 +583,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -560,10 +597,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -585,10 +622,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -596,10 +633,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -607,13 +641,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -621,13 +655,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -635,13 +669,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,13 +683,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,13 +697,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -677,10 +711,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,13 +722,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -702,13 +736,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -716,13 +750,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,13 +764,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -744,10 +778,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -755,10 +789,117 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
         <v>41</v>
       </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -768,58 +909,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
- Agregamos mas items al backlog
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>Entender ejemplo Ruby</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>Mejorar css</t>
+  </si>
+  <si>
+    <t>Prioridad</t>
+  </si>
+  <si>
+    <t>Cada perfil tiene un tipo de intervalo entre preguntas y cuando valen las respuestas</t>
   </si>
 </sst>
 </file>
@@ -234,10 +240,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -540,371 +548,427 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="D17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="D18" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>9</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>10</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="B25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>14</v>
       </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="B26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>15</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>16</v>
       </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" t="s">
-        <v>52</v>
+      <c r="D28" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>35</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E29">
+    <sortCondition ref="E2:E29"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="B6" location="'Agregar jugadores'!A1" display="Poder agregar jugadores"/>
+    <hyperlink ref="B18" location="'Agregar jugadores'!A1" display="Poder agregar jugadores"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ahora se puede manejar el estado del juego desde afuera
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Entender ejemplo Ruby</t>
   </si>
@@ -551,7 +551,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,6 +586,9 @@
       <c r="C2" t="s">
         <v>43</v>
       </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
       <c r="E2">
         <v>1</v>
       </c>
@@ -599,6 +602,9 @@
       </c>
       <c r="C3" t="s">
         <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
       <c r="E3">
         <v>2</v>

</xml_diff>

<commit_message>
Se agrego una configuracion de niveles
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
   <si>
     <t>Entender ejemplo Ruby</t>
   </si>
@@ -188,6 +188,15 @@
   </si>
   <si>
     <t>Cada perfil tiene un tipo de intervalo entre preguntas y cuando valen las respuestas</t>
+  </si>
+  <si>
+    <t>Incrementar/decrementar puntajes</t>
+  </si>
+  <si>
+    <t>Según la configuración del perfil</t>
+  </si>
+  <si>
+    <t>En una página con botones para elegir el perfil</t>
   </si>
 </sst>
 </file>
@@ -548,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +629,9 @@
       <c r="C4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E4">
         <v>3</v>
       </c>
@@ -635,6 +646,9 @@
       <c r="C5" t="s">
         <v>41</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E5">
         <v>3</v>
       </c>
@@ -649,44 +663,51 @@
       <c r="C6" t="s">
         <v>47</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E6">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="2"/>
       <c r="E7">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -694,110 +715,110 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E12">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>50</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>4</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14">
-        <v>9999999</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15">
+        <v>9999999</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>9</v>
@@ -805,13 +826,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>5</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>9</v>
@@ -819,13 +840,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>7</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
@@ -833,13 +854,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>9</v>
@@ -847,13 +868,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>9</v>
@@ -861,13 +882,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>9</v>
@@ -875,13 +896,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>9</v>
@@ -889,39 +910,39 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="D24" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>9</v>
@@ -929,13 +950,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>9</v>
@@ -943,29 +964,43 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
+        <v>15</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>16</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="D29" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>18</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>34</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -974,7 +1009,7 @@
     <sortCondition ref="E2:E29"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B18" location="'Agregar jugadores'!A1" display="Poder agregar jugadores"/>
+    <hyperlink ref="B19" location="'Agregar jugadores'!A1" display="Poder agregar jugadores"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregamos el cambio de nivel en runtime
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+  <si>
+    <t>ok</t>
+  </si>
   <si>
     <t>To do</t>
   </si>
@@ -447,7 +450,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,42 +464,44 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -504,25 +509,25 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -530,10 +535,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -541,7 +546,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -549,24 +554,24 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -574,10 +579,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -585,10 +590,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -596,10 +601,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D12">
         <v>11</v>

</xml_diff>

<commit_message>
Se agrego el "paso"
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>ok</t>
   </si>
@@ -97,7 +97,7 @@
     <t>Adrián</t>
   </si>
   <si>
-    <t>Diego</t>
+    <t>Diego e Iván</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,8 +503,14 @@
       <c r="B3" t="s">
         <v>12</v>
       </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
       <c r="D3">
         <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Arregle un bug y agregue una preguntas como JSON
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>ok</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Diego e Iván</t>
+  </si>
+  <si>
+    <t>Adrián y Diego</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +528,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -535,8 +538,14 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="D5">
         <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se agrego una pagina de administracion
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>ok</t>
   </si>
@@ -574,6 +574,9 @@
       <c r="B8" t="s">
         <v>11</v>
       </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
       <c r="D8">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Ahora los puntajes no descienden de 0
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>ok</t>
   </si>
@@ -453,7 +453,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +523,9 @@
       <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="D4">
         <v>3</v>
       </c>
@@ -562,6 +564,9 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
       </c>
       <c r="D7">
         <v>6</v>

</xml_diff>

<commit_message>
El leaderboard muestra la ultima pregunta ok
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>ok</t>
   </si>
@@ -453,7 +453,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,6 +557,9 @@
       <c r="B6" t="s">
         <v>15</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="D6">
         <v>5</v>
       </c>
@@ -595,6 +598,9 @@
       </c>
       <c r="B9" t="s">
         <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
       </c>
       <c r="D9">
         <v>8</v>

</xml_diff>

<commit_message>
Se cambiaron los nombres de los estados
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>ok</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Adrián y Diego</t>
+  </si>
+  <si>
+    <t>Diego</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,6 +566,9 @@
       <c r="D6">
         <v>5</v>
       </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -574,6 +580,9 @@
       <c r="D7">
         <v>6</v>
       </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -605,6 +614,9 @@
       <c r="D9">
         <v>8</v>
       </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -613,8 +625,14 @@
       <c r="B10" t="s">
         <v>17</v>
       </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
       <c r="D10">
         <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>